<commit_message>
Added additional line item to run for multi data
</commit_message>
<xml_diff>
--- a/data/TC001.xlsx
+++ b/data/TC001.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E85675-E24A-4D2A-9145-4AB824BE5D9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7BFC4B-E105-4454-90C0-8385F943E08C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Amount</t>
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>120</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,6 +445,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>